<commit_message>
file duplicate in the andorid andiphone...
</commit_message>
<xml_diff>
--- a/matrix/executed/app/iPhone/login_password_execute.xlsx
+++ b/matrix/executed/app/iPhone/login_password_execute.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08DB0E2-65AE-44FC-BE9C-02D0CEA1DF4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\matrix\reviewed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE1E18D-F24A-4C5E-A625-9E2EC727F37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login_password" sheetId="1" r:id="rId1"/>
+    <sheet name="reviewed_connection_page" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>T001</t>
   </si>
@@ -55,6 +57,9 @@
     <t>T0010</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>T0011</t>
   </si>
   <si>
@@ -65,39 +70,6 @@
   </si>
   <si>
     <t>T0014</t>
-  </si>
-  <si>
-    <t>T0015</t>
-  </si>
-  <si>
-    <t>T0016</t>
-  </si>
-  <si>
-    <t>T0017</t>
-  </si>
-  <si>
-    <t>T0018</t>
-  </si>
-  <si>
-    <t>T0019</t>
-  </si>
-  <si>
-    <t>T0020</t>
-  </si>
-  <si>
-    <t>T0021</t>
-  </si>
-  <si>
-    <t>T0022</t>
-  </si>
-  <si>
-    <t>T0023</t>
-  </si>
-  <si>
-    <t>T0024</t>
-  </si>
-  <si>
-    <t>T0025</t>
   </si>
 </sst>
 </file>
@@ -227,7 +199,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -267,27 +239,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -325,25 +277,25 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
+                  <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E2E661-D141-4EBE-A1B9-A191333CB81D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -392,25 +344,25 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
+                  <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F963AF5D-DE04-471C-81B3-1C64B171ACD9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -456,28 +408,23 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
+                  <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C216D670-5A9E-42CA-B9EA-DD9252B43797}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EC2FB5A-C238-4C6F-8961-D2EBF3BC08FE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -517,34 +464,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
+                  <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5F6470-F599-4B57-A0CF-3B6F278A2D84}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8293D954-4250-4ECA-A89A-5058669F18CC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -584,34 +526,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
+                  <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E227688-DBC9-47A4-88E2-308E76C996E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17146D7A-34D6-45D7-BA2F-7C6868999ED4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -651,34 +588,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1030"/>
+                  <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE2F6A5-2E16-4895-865F-5374C5CA9FAD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0D49ADA-E474-4F19-90AC-7405D6407A97}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -718,34 +650,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1031"/>
+                  <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C825FA37-6BAB-4684-8AF9-05B97D2A0056}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5931AB4E-AE31-40B0-BA6B-36A67DF97F65}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -785,34 +712,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1032"/>
+                  <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7884DB1-918B-4C3B-A092-5121625B9E29}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F9E4D4-7013-4E58-B34A-0EFDE9BAB1F4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -852,34 +774,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1033"/>
+                  <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7707766E-3848-4031-B918-C606FEB1852C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56DB7D99-BF18-4948-9963-6397C534972E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -919,34 +836,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
+            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1034"/>
+                  <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73B2B74A-4D75-49F0-8E56-A39263F685EA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3182C70-53DB-4E14-BE47-681135563BB9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -986,34 +898,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
+            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1035"/>
+                  <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7E72568-244C-4AC7-BC54-F0C7EF09266C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F24153-11C4-43F4-B8A7-33D2376F2033}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1053,34 +960,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
+            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1036"/>
+                  <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46246F26-815F-4ABE-AB33-7E6FCB8DD40F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A3BA9C7-7B3A-44E1-A013-B85567D1D4BD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1120,34 +1022,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
+            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1037"/>
+                  <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B146ED4-A430-44C0-B02D-81697E89CB4B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87BC3330-E8EB-41C9-A508-368E8FB133E4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1187,34 +1084,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
+            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1038"/>
+                  <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3097235-964C-43A3-B4EA-8A11B21266B3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4931E553-DA06-4038-BD32-B10F9B46307B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1254,34 +1146,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>14</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>0</xdr:row>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>14</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1039"/>
+                  <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3148EE0-69B3-40DB-B10C-9C3D75636AE2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01D21E22-2A0E-469D-91B9-6A621CC7D408}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1321,34 +1208,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1040"/>
+                  <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA3AB50E-1736-4DF4-ACEC-03E0FAF59264}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC435E2-35F3-433B-90A5-291B8FC80382}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1388,34 +1270,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1041"/>
+                  <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE06ED00-3041-4E78-B2C1-CC0E4B0BF254}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF28EE06-1385-404C-9235-CF293718CEC1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1455,34 +1332,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1042"/>
+                  <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE2E7DD-7A9D-4C0C-B6C6-85EE9EA61C05}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF3683F2-7BFB-4F61-B2C1-30F214EC2B37}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1522,34 +1394,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1043"/>
+                  <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8ABBAFF-6C3F-4CFD-9652-DA9CC66550A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51039C51-B31E-4E9C-A4AB-4A76845414ED}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1589,34 +1456,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1044"/>
+                  <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE932C94-48B0-4924-B423-C65D94523FAA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1753B809-3739-4A0B-A552-3964F66BE7FF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1656,34 +1518,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
+            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1045"/>
+                  <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F5C016-E68A-438A-A8F7-86BE65470756}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9F0B59-0972-4905-B919-CE6B67AF3017}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1723,34 +1580,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
+            <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1046"/>
+                  <a14:compatExt spid="_x0000_s1049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D27BB5E7-9BC9-4A90-800B-ACAD4AFFA105}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35A56385-903F-4431-9255-23A52DC5868C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1790,34 +1642,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>15</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
+            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1047"/>
+                  <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29BED4F4-A428-40F9-A17D-D87F595CC00A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866458E6-0632-42E0-9284-180E26BCA9BC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1857,34 +1704,29 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>167640</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="396240" cy="281940"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
+            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1048"/>
+                  <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13724131-4269-42B2-AAB0-F216F89639E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6786BEB-EA73-4A26-A883-654643821684}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1924,342 +1766,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>11</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C216226-E96A-496A-955C-D589968DB808}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE40670-CB4C-4D05-8056-6FE2D67C9BC4}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3FB4C5-6E5A-468D-9E6B-47E72D033744}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1052"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40E3B083-3DAC-452E-A8E6-D85B35D4E586}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1053"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9089A0-FE6B-4088-BF60-17F1FE929B29}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2529,115 +2036,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3">
-        <v>45307</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
+    </row>
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>45246</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2651,6 +2114,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2661,19 +2125,19 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId3" name="Check Box 1">
+            <control shapeId="1027" r:id="rId3" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2683,19 +2147,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+            <control shapeId="1029" r:id="rId4" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId5" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>91440</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2705,19 +2191,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId5" name="Check Box 3">
+            <control shapeId="1031" r:id="rId6" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2727,19 +2213,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId6" name="Check Box 4">
+            <control shapeId="1032" r:id="rId7" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2749,19 +2235,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId7" name="Check Box 5">
+            <control shapeId="1033" r:id="rId8" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1034" r:id="rId9" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2771,19 +2279,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId8" name="Check Box 6">
+            <control shapeId="1035" r:id="rId10" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>7</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2793,19 +2301,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId9" name="Check Box 7">
+            <control shapeId="1036" r:id="rId11" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2815,19 +2323,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId10" name="Check Box 8">
+            <control shapeId="1037" r:id="rId12" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1038" r:id="rId13" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2837,19 +2367,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId11" name="Check Box 9">
+            <control shapeId="1039" r:id="rId14" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2859,19 +2389,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId12" name="Check Box 10">
+            <control shapeId="1040" r:id="rId15" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>11</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>11</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2881,19 +2411,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId13" name="Check Box 11">
+            <control shapeId="1041" r:id="rId16" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1042" r:id="rId17" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2903,19 +2455,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId14" name="Check Box 12">
+            <control shapeId="1043" r:id="rId18" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>13</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>13</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2925,19 +2477,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId15" name="Check Box 13">
+            <control shapeId="1044" r:id="rId19" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2947,19 +2499,41 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId16" name="Check Box 14">
+            <control shapeId="1045" r:id="rId20" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>144780</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1046" r:id="rId21" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2969,19 +2543,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId17" name="Check Box 15">
+            <control shapeId="1047" r:id="rId22" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>14</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>0</xdr:row>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
+                    <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>14</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>2</xdr:row>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2991,20 +2565,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId18" name="Check Box 16">
+            <control shapeId="1048" r:id="rId23" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:col>14</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>14</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3013,20 +2587,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId19" name="Check Box 17">
+            <control shapeId="1049" r:id="rId24" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3035,20 +2609,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId20" name="Check Box 18">
+            <control shapeId="1050" r:id="rId25" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>15</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3057,240 +2631,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId21" name="Check Box 19">
+            <control shapeId="1051" r:id="rId26" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>167640</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>563880</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId22" name="Check Box 20">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId23" name="Check Box 21">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId24" name="Check Box 22">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>8</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId25" name="Check Box 23">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>9</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>9</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId26" name="Check Box 24">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>10</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>10</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId27" name="Check Box 25">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>11</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>11</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId28" name="Check Box 26">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId29" name="Check Box 27">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId30" name="Check Box 28">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>12</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId31" name="Check Box 29">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>171450</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>